<commit_message>
Updated standby altimeter and airspeed/vvi gauge PCBs
</commit_message>
<xml_diff>
--- a/ECAD/PCBs/ABSIS/ABSIS_BOM.xlsx
+++ b/ECAD/PCBs/ABSIS/ABSIS_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OpenHornet\ECAD\PCBs\ABSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF18B90B-4BA8-4B4F-ACBE-ABA1D4EC14D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C7C084-69C2-4C91-A4C2-72B33FCB2CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="-15465" windowWidth="21600" windowHeight="11385" xr2:uid="{B0783D0E-82DA-4DF1-8333-2522E986E31D}"/>
   </bookViews>
@@ -170,9 +170,6 @@
     <t>QTY</t>
   </si>
   <si>
-    <t>ABSIS ALE Relay Module</t>
-  </si>
-  <si>
     <t>J3, J4</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samtec-inc/SSQ-116-03-T-D/1111844</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -268,12 +268,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -289,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +311,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,7 +631,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,35 +674,35 @@
         <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -704,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I3">
         <v>1.27</v>
@@ -727,12 +741,12 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -742,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -764,7 +778,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -796,7 +810,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -828,7 +842,7 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -838,13 +852,13 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7">
         <v>0.27</v>
@@ -865,7 +879,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -897,29 +911,29 @@
         <v>44</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -929,13 +943,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>3.16</v>
@@ -958,12 +972,12 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -994,12 +1008,12 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1030,12 +1044,12 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1066,12 +1080,12 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="4" t="s">

</xml_diff>

<commit_message>
LIP Interconnect Work Continues
</commit_message>
<xml_diff>
--- a/ECAD/PCBs/ABSIS/ABSIS_BOM.xlsx
+++ b/ECAD/PCBs/ABSIS/ABSIS_BOM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OpenHornet\ECAD\PCBs\ABSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E438F87-B6BF-4289-A2BC-967361893131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6065E635-3DDF-4656-AB58-0471E44F2AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{B0783D0E-82DA-4DF1-8333-2522E986E31D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B0783D0E-82DA-4DF1-8333-2522E986E31D}"/>
   </bookViews>
   <sheets>
     <sheet name="TH Components" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -631,7 +632,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="C7" activeCellId="2" sqref="C4:C6 C10 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +747,7 @@
       <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -810,7 +811,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -842,7 +843,7 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -933,7 +934,7 @@
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">

</xml_diff>